<commit_message>
skoro konec Vltavy :)
vekt hotova, jen se musi dodelat topo
</commit_message>
<xml_diff>
--- a/hodiny.xlsx
+++ b/hodiny.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E250F2-A6DA-4AA3-A87D-A3331141BDC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DE072B-E7F0-46C8-9317-B67BE86CA58E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="4650" windowWidth="28800" windowHeight="14925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>čas [min]</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>31.7.</t>
+  </si>
+  <si>
+    <t>2.8.</t>
+  </si>
+  <si>
+    <t>3.8.</t>
+  </si>
+  <si>
+    <t>12.8.</t>
   </si>
 </sst>
 </file>
@@ -688,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K126" sqref="K126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4297,171 +4306,208 @@
       </c>
     </row>
     <row r="126" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C126" s="2"/>
-      <c r="D126" s="10"/>
+      <c r="B126" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C126" s="2">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D126" s="10">
+        <v>0.53749999999999998</v>
+      </c>
       <c r="E126" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3.4027777777777768E-2</v>
       </c>
       <c r="F126" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>3.9499999999999988</v>
       </c>
       <c r="G126" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>3.9499999999999988</v>
       </c>
       <c r="H126" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I126" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>20808</v>
       </c>
     </row>
     <row r="127" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C127" s="2"/>
-      <c r="D127" s="10"/>
+      <c r="B127" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C127" s="2">
+        <v>0.29305555555555557</v>
+      </c>
+      <c r="D127" s="10">
+        <v>0.3263888888888889</v>
+      </c>
       <c r="E127" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3.3333333333333326E-2</v>
       </c>
       <c r="F127" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>3.9833333333333321</v>
       </c>
       <c r="G127" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>3.9833333333333321</v>
       </c>
       <c r="H127" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.1333333333333329</v>
       </c>
       <c r="I127" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>20943.999999999996</v>
       </c>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C128" s="2"/>
-      <c r="D128" s="10"/>
+      <c r="B128" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C128" s="2">
+        <v>0.53541666666666665</v>
+      </c>
+      <c r="D128" s="10">
+        <v>0.54999999999999993</v>
+      </c>
       <c r="E128" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1.4583333333333282E-2</v>
       </c>
       <c r="F128" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>3.9979166666666655</v>
       </c>
       <c r="G128" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>3.9979166666666655</v>
       </c>
       <c r="H128" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.1479166666666654</v>
       </c>
       <c r="I128" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>21003.499999999996</v>
       </c>
     </row>
     <row r="129" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C129" s="2"/>
-      <c r="D129" s="10"/>
+      <c r="C129" s="2">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="D129" s="10">
+        <v>0.57152777777777775</v>
+      </c>
       <c r="E129" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1.7361111111111049E-2</v>
       </c>
       <c r="F129" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.0152777777777766</v>
       </c>
       <c r="G129" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.0152777777777766</v>
       </c>
       <c r="H129" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.1652777777777779</v>
       </c>
       <c r="I129" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>21074.333333333332</v>
       </c>
     </row>
     <row r="130" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C130" s="2"/>
-      <c r="D130" s="10"/>
+      <c r="C130" s="2">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D130" s="10">
+        <v>0.77916666666666667</v>
+      </c>
       <c r="E130" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>0.12638888888888888</v>
       </c>
       <c r="F130" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.1416666666666657</v>
       </c>
       <c r="G130" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.1416666666666657</v>
       </c>
       <c r="H130" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.291666666666667</v>
       </c>
       <c r="I130" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>21590</v>
       </c>
     </row>
     <row r="131" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C131" s="2"/>
-      <c r="D131" s="10"/>
+      <c r="C131" s="2">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D131" s="10">
+        <v>0.83819444444444446</v>
+      </c>
       <c r="E131" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>4.9999999999999933E-2</v>
       </c>
       <c r="F131" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.1916666666666655</v>
       </c>
       <c r="G131" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.1916666666666655</v>
       </c>
       <c r="H131" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.3416666666666668</v>
       </c>
       <c r="I131" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>21793.999999999996</v>
       </c>
     </row>
     <row r="132" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C132" s="2"/>
-      <c r="D132" s="10"/>
+      <c r="C132" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D132" s="10">
+        <v>0.95138888888888884</v>
+      </c>
       <c r="E132" s="12">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>5.5555555555555469E-2</v>
       </c>
       <c r="F132" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G132" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H132" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I132" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="133" spans="3:9" x14ac:dyDescent="0.25">
@@ -4473,19 +4519,19 @@
       </c>
       <c r="F133" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G133" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H133" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I133" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="134" spans="3:9" x14ac:dyDescent="0.25">
@@ -4497,19 +4543,19 @@
       </c>
       <c r="F134" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G134" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H134" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I134" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="135" spans="3:9" x14ac:dyDescent="0.25">
@@ -4521,19 +4567,19 @@
       </c>
       <c r="F135" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G135" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H135" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I135" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="136" spans="3:9" x14ac:dyDescent="0.25">
@@ -4545,19 +4591,19 @@
       </c>
       <c r="F136" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G136" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H136" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I136" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="137" spans="3:9" x14ac:dyDescent="0.25">
@@ -4569,19 +4615,19 @@
       </c>
       <c r="F137" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G137" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H137" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I137" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="138" spans="3:9" x14ac:dyDescent="0.25">
@@ -4593,19 +4639,19 @@
       </c>
       <c r="F138" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G138" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H138" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I138" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="139" spans="3:9" x14ac:dyDescent="0.25">
@@ -4617,19 +4663,19 @@
       </c>
       <c r="F139" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G139" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H139" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I139" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="140" spans="3:9" x14ac:dyDescent="0.25">
@@ -4641,19 +4687,19 @@
       </c>
       <c r="F140" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G140" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H140" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I140" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="141" spans="3:9" x14ac:dyDescent="0.25">
@@ -4665,19 +4711,19 @@
       </c>
       <c r="F141" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G141" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H141" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I141" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="142" spans="3:9" x14ac:dyDescent="0.25">
@@ -4689,19 +4735,19 @@
       </c>
       <c r="F142" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G142" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H142" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I142" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="143" spans="3:9" x14ac:dyDescent="0.25">
@@ -4713,19 +4759,19 @@
       </c>
       <c r="F143" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G143" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H143" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I143" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="144" spans="3:9" x14ac:dyDescent="0.25">
@@ -4737,19 +4783,19 @@
       </c>
       <c r="F144" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G144" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H144" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I144" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="145" spans="3:9" x14ac:dyDescent="0.25">
@@ -4761,19 +4807,19 @@
       </c>
       <c r="F145" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G145" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H145" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I145" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="146" spans="3:9" x14ac:dyDescent="0.25">
@@ -4785,19 +4831,19 @@
       </c>
       <c r="F146" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G146" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H146" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I146" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="147" spans="3:9" x14ac:dyDescent="0.25">
@@ -4809,19 +4855,19 @@
       </c>
       <c r="F147" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G147" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H147" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I147" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="148" spans="3:9" x14ac:dyDescent="0.25">
@@ -4833,19 +4879,19 @@
       </c>
       <c r="F148" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G148" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H148" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I148" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="149" spans="3:9" x14ac:dyDescent="0.25">
@@ -4857,19 +4903,19 @@
       </c>
       <c r="F149" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G149" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H149" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I149" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="150" spans="3:9" x14ac:dyDescent="0.25">
@@ -4881,19 +4927,19 @@
       </c>
       <c r="F150" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G150" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H150" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I150" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="151" spans="3:9" x14ac:dyDescent="0.25">
@@ -4905,19 +4951,19 @@
       </c>
       <c r="F151" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G151" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H151" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I151" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="152" spans="3:9" x14ac:dyDescent="0.25">
@@ -4929,19 +4975,19 @@
       </c>
       <c r="F152" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G152" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H152" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I152" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="153" spans="3:9" x14ac:dyDescent="0.25">
@@ -4953,19 +4999,19 @@
       </c>
       <c r="F153" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G153" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H153" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I153" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="154" spans="3:9" x14ac:dyDescent="0.25">
@@ -4977,19 +5023,19 @@
       </c>
       <c r="F154" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G154" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H154" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I154" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="155" spans="3:9" x14ac:dyDescent="0.25">
@@ -5001,19 +5047,19 @@
       </c>
       <c r="F155" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G155" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H155" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I155" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="156" spans="3:9" x14ac:dyDescent="0.25">
@@ -5025,19 +5071,19 @@
       </c>
       <c r="F156" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G156" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H156" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I156" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="157" spans="3:9" x14ac:dyDescent="0.25">
@@ -5049,19 +5095,19 @@
       </c>
       <c r="F157" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G157" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H157" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I157" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="158" spans="3:9" x14ac:dyDescent="0.25">
@@ -5073,19 +5119,19 @@
       </c>
       <c r="F158" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G158" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H158" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I158" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="159" spans="3:9" x14ac:dyDescent="0.25">
@@ -5097,19 +5143,19 @@
       </c>
       <c r="F159" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G159" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H159" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I159" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="160" spans="3:9" x14ac:dyDescent="0.25">
@@ -5121,19 +5167,19 @@
       </c>
       <c r="F160" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G160" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H160" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I160" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="161" spans="3:9" x14ac:dyDescent="0.25">
@@ -5145,19 +5191,19 @@
       </c>
       <c r="F161" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G161" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H161" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I161" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="162" spans="3:9" x14ac:dyDescent="0.25">
@@ -5169,19 +5215,19 @@
       </c>
       <c r="F162" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G162" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H162" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I162" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="163" spans="3:9" x14ac:dyDescent="0.25">
@@ -5193,19 +5239,19 @@
       </c>
       <c r="F163" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G163" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H163" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I163" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="164" spans="3:9" x14ac:dyDescent="0.25">
@@ -5217,19 +5263,19 @@
       </c>
       <c r="F164" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G164" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H164" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I164" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="165" spans="3:9" x14ac:dyDescent="0.25">
@@ -5241,19 +5287,19 @@
       </c>
       <c r="F165" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G165" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H165" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I165" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="166" spans="3:9" x14ac:dyDescent="0.25">
@@ -5265,19 +5311,19 @@
       </c>
       <c r="F166" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G166" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H166" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I166" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="167" spans="3:9" x14ac:dyDescent="0.25">
@@ -5289,19 +5335,19 @@
       </c>
       <c r="F167" s="13">
         <f t="shared" si="15"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G167" s="8">
         <f t="shared" si="16"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H167" s="8">
         <f t="shared" si="17"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I167" s="15">
         <f t="shared" si="18"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="168" spans="3:9" x14ac:dyDescent="0.25">
@@ -5313,19 +5359,19 @@
       </c>
       <c r="F168" s="13">
         <f t="shared" ref="F168:F231" si="20">F167+E168</f>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G168" s="8">
         <f t="shared" ref="G168:G231" si="21">F168</f>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H168" s="8">
         <f t="shared" ref="H168:H231" si="22">(H167+G168-G167)</f>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I168" s="15">
         <f t="shared" ref="I168:I231" si="23">H168*24*$J$2</f>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="169" spans="3:9" x14ac:dyDescent="0.25">
@@ -5337,19 +5383,19 @@
       </c>
       <c r="F169" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G169" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H169" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I169" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="170" spans="3:9" x14ac:dyDescent="0.25">
@@ -5361,19 +5407,19 @@
       </c>
       <c r="F170" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G170" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H170" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I170" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="171" spans="3:9" x14ac:dyDescent="0.25">
@@ -5385,19 +5431,19 @@
       </c>
       <c r="F171" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G171" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H171" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I171" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="172" spans="3:9" x14ac:dyDescent="0.25">
@@ -5409,19 +5455,19 @@
       </c>
       <c r="F172" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G172" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H172" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I172" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="173" spans="3:9" x14ac:dyDescent="0.25">
@@ -5433,19 +5479,19 @@
       </c>
       <c r="F173" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G173" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H173" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I173" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="174" spans="3:9" x14ac:dyDescent="0.25">
@@ -5457,19 +5503,19 @@
       </c>
       <c r="F174" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G174" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H174" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I174" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="175" spans="3:9" x14ac:dyDescent="0.25">
@@ -5481,19 +5527,19 @@
       </c>
       <c r="F175" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G175" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H175" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I175" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="176" spans="3:9" x14ac:dyDescent="0.25">
@@ -5505,19 +5551,19 @@
       </c>
       <c r="F176" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G176" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H176" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I176" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="177" spans="3:9" x14ac:dyDescent="0.25">
@@ -5529,19 +5575,19 @@
       </c>
       <c r="F177" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G177" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H177" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I177" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="178" spans="3:9" x14ac:dyDescent="0.25">
@@ -5553,19 +5599,19 @@
       </c>
       <c r="F178" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G178" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H178" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I178" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="179" spans="3:9" x14ac:dyDescent="0.25">
@@ -5577,19 +5623,19 @@
       </c>
       <c r="F179" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G179" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H179" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I179" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="180" spans="3:9" x14ac:dyDescent="0.25">
@@ -5601,19 +5647,19 @@
       </c>
       <c r="F180" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G180" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H180" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I180" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="181" spans="3:9" x14ac:dyDescent="0.25">
@@ -5625,19 +5671,19 @@
       </c>
       <c r="F181" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G181" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H181" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I181" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="182" spans="3:9" x14ac:dyDescent="0.25">
@@ -5649,19 +5695,19 @@
       </c>
       <c r="F182" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G182" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H182" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I182" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="183" spans="3:9" x14ac:dyDescent="0.25">
@@ -5673,19 +5719,19 @@
       </c>
       <c r="F183" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G183" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H183" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I183" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="184" spans="3:9" x14ac:dyDescent="0.25">
@@ -5697,19 +5743,19 @@
       </c>
       <c r="F184" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G184" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H184" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I184" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="185" spans="3:9" x14ac:dyDescent="0.25">
@@ -5721,19 +5767,19 @@
       </c>
       <c r="F185" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G185" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H185" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I185" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="186" spans="3:9" x14ac:dyDescent="0.25">
@@ -5745,19 +5791,19 @@
       </c>
       <c r="F186" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G186" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H186" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I186" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="187" spans="3:9" x14ac:dyDescent="0.25">
@@ -5769,19 +5815,19 @@
       </c>
       <c r="F187" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G187" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H187" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I187" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="188" spans="3:9" x14ac:dyDescent="0.25">
@@ -5793,19 +5839,19 @@
       </c>
       <c r="F188" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G188" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H188" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I188" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="189" spans="3:9" x14ac:dyDescent="0.25">
@@ -5817,19 +5863,19 @@
       </c>
       <c r="F189" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G189" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H189" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I189" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="190" spans="3:9" x14ac:dyDescent="0.25">
@@ -5841,19 +5887,19 @@
       </c>
       <c r="F190" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G190" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H190" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I190" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="191" spans="3:9" x14ac:dyDescent="0.25">
@@ -5865,19 +5911,19 @@
       </c>
       <c r="F191" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G191" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H191" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I191" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="192" spans="3:9" x14ac:dyDescent="0.25">
@@ -5889,19 +5935,19 @@
       </c>
       <c r="F192" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G192" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H192" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I192" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="193" spans="3:9" x14ac:dyDescent="0.25">
@@ -5913,19 +5959,19 @@
       </c>
       <c r="F193" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G193" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H193" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I193" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="194" spans="3:9" x14ac:dyDescent="0.25">
@@ -5937,19 +5983,19 @@
       </c>
       <c r="F194" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G194" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H194" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I194" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="195" spans="3:9" x14ac:dyDescent="0.25">
@@ -5961,19 +6007,19 @@
       </c>
       <c r="F195" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G195" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H195" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I195" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="196" spans="3:9" x14ac:dyDescent="0.25">
@@ -5985,19 +6031,19 @@
       </c>
       <c r="F196" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G196" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H196" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I196" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="197" spans="3:9" x14ac:dyDescent="0.25">
@@ -6009,19 +6055,19 @@
       </c>
       <c r="F197" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G197" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H197" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I197" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="198" spans="3:9" x14ac:dyDescent="0.25">
@@ -6033,19 +6079,19 @@
       </c>
       <c r="F198" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G198" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H198" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I198" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="199" spans="3:9" x14ac:dyDescent="0.25">
@@ -6057,19 +6103,19 @@
       </c>
       <c r="F199" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G199" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H199" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I199" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="200" spans="3:9" x14ac:dyDescent="0.25">
@@ -6081,19 +6127,19 @@
       </c>
       <c r="F200" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G200" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H200" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I200" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="201" spans="3:9" x14ac:dyDescent="0.25">
@@ -6105,19 +6151,19 @@
       </c>
       <c r="F201" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G201" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H201" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I201" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="202" spans="3:9" x14ac:dyDescent="0.25">
@@ -6129,19 +6175,19 @@
       </c>
       <c r="F202" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G202" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H202" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I202" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="203" spans="3:9" x14ac:dyDescent="0.25">
@@ -6153,19 +6199,19 @@
       </c>
       <c r="F203" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G203" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H203" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I203" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="204" spans="3:9" x14ac:dyDescent="0.25">
@@ -6177,19 +6223,19 @@
       </c>
       <c r="F204" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G204" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H204" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I204" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="205" spans="3:9" x14ac:dyDescent="0.25">
@@ -6201,19 +6247,19 @@
       </c>
       <c r="F205" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G205" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H205" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I205" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="206" spans="3:9" x14ac:dyDescent="0.25">
@@ -6225,19 +6271,19 @@
       </c>
       <c r="F206" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G206" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H206" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I206" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="207" spans="3:9" x14ac:dyDescent="0.25">
@@ -6249,19 +6295,19 @@
       </c>
       <c r="F207" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G207" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H207" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I207" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="208" spans="3:9" x14ac:dyDescent="0.25">
@@ -6273,19 +6319,19 @@
       </c>
       <c r="F208" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G208" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H208" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I208" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="209" spans="3:9" x14ac:dyDescent="0.25">
@@ -6297,19 +6343,19 @@
       </c>
       <c r="F209" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G209" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H209" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I209" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="210" spans="3:9" x14ac:dyDescent="0.25">
@@ -6321,19 +6367,19 @@
       </c>
       <c r="F210" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G210" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H210" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I210" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="211" spans="3:9" x14ac:dyDescent="0.25">
@@ -6345,19 +6391,19 @@
       </c>
       <c r="F211" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G211" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H211" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I211" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="212" spans="3:9" x14ac:dyDescent="0.25">
@@ -6369,19 +6415,19 @@
       </c>
       <c r="F212" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G212" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H212" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I212" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="213" spans="3:9" x14ac:dyDescent="0.25">
@@ -6393,19 +6439,19 @@
       </c>
       <c r="F213" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G213" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H213" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I213" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="214" spans="3:9" x14ac:dyDescent="0.25">
@@ -6417,19 +6463,19 @@
       </c>
       <c r="F214" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G214" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H214" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I214" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="215" spans="3:9" x14ac:dyDescent="0.25">
@@ -6441,19 +6487,19 @@
       </c>
       <c r="F215" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G215" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H215" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I215" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="216" spans="3:9" x14ac:dyDescent="0.25">
@@ -6465,19 +6511,19 @@
       </c>
       <c r="F216" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G216" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H216" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I216" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="217" spans="3:9" x14ac:dyDescent="0.25">
@@ -6489,19 +6535,19 @@
       </c>
       <c r="F217" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G217" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H217" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I217" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="218" spans="3:9" x14ac:dyDescent="0.25">
@@ -6513,19 +6559,19 @@
       </c>
       <c r="F218" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G218" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H218" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I218" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="219" spans="3:9" x14ac:dyDescent="0.25">
@@ -6537,19 +6583,19 @@
       </c>
       <c r="F219" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G219" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H219" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I219" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="220" spans="3:9" x14ac:dyDescent="0.25">
@@ -6561,19 +6607,19 @@
       </c>
       <c r="F220" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G220" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H220" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I220" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="221" spans="3:9" x14ac:dyDescent="0.25">
@@ -6585,19 +6631,19 @@
       </c>
       <c r="F221" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G221" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H221" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I221" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="222" spans="3:9" x14ac:dyDescent="0.25">
@@ -6609,19 +6655,19 @@
       </c>
       <c r="F222" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G222" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H222" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I222" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="223" spans="3:9" x14ac:dyDescent="0.25">
@@ -6633,19 +6679,19 @@
       </c>
       <c r="F223" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G223" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H223" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I223" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="224" spans="3:9" x14ac:dyDescent="0.25">
@@ -6657,19 +6703,19 @@
       </c>
       <c r="F224" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G224" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H224" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I224" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="225" spans="3:9" x14ac:dyDescent="0.25">
@@ -6681,19 +6727,19 @@
       </c>
       <c r="F225" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G225" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H225" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I225" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="226" spans="3:9" x14ac:dyDescent="0.25">
@@ -6705,19 +6751,19 @@
       </c>
       <c r="F226" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G226" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H226" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I226" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="227" spans="3:9" x14ac:dyDescent="0.25">
@@ -6729,19 +6775,19 @@
       </c>
       <c r="F227" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G227" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H227" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I227" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="228" spans="3:9" x14ac:dyDescent="0.25">
@@ -6753,19 +6799,19 @@
       </c>
       <c r="F228" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G228" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H228" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I228" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="229" spans="3:9" x14ac:dyDescent="0.25">
@@ -6777,19 +6823,19 @@
       </c>
       <c r="F229" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G229" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H229" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I229" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="230" spans="3:9" x14ac:dyDescent="0.25">
@@ -6801,19 +6847,19 @@
       </c>
       <c r="F230" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G230" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H230" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I230" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="231" spans="3:9" x14ac:dyDescent="0.25">
@@ -6825,19 +6871,19 @@
       </c>
       <c r="F231" s="13">
         <f t="shared" si="20"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G231" s="8">
         <f t="shared" si="21"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H231" s="8">
         <f t="shared" si="22"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I231" s="15">
         <f t="shared" si="23"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="232" spans="3:9" x14ac:dyDescent="0.25">
@@ -6849,19 +6895,19 @@
       </c>
       <c r="F232" s="13">
         <f t="shared" ref="F232:F255" si="25">F231+E232</f>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G232" s="8">
         <f t="shared" ref="G232:G255" si="26">F232</f>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H232" s="8">
         <f t="shared" ref="H232:H255" si="27">(H231+G232-G231)</f>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I232" s="15">
         <f t="shared" ref="I232:I255" si="28">H232*24*$J$2</f>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="233" spans="3:9" x14ac:dyDescent="0.25">
@@ -6873,19 +6919,19 @@
       </c>
       <c r="F233" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G233" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H233" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I233" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="234" spans="3:9" x14ac:dyDescent="0.25">
@@ -6897,19 +6943,19 @@
       </c>
       <c r="F234" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G234" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H234" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I234" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="235" spans="3:9" x14ac:dyDescent="0.25">
@@ -6921,19 +6967,19 @@
       </c>
       <c r="F235" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G235" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H235" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I235" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="236" spans="3:9" x14ac:dyDescent="0.25">
@@ -6945,19 +6991,19 @@
       </c>
       <c r="F236" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G236" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H236" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I236" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="237" spans="3:9" x14ac:dyDescent="0.25">
@@ -6969,19 +7015,19 @@
       </c>
       <c r="F237" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G237" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H237" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I237" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="238" spans="3:9" x14ac:dyDescent="0.25">
@@ -6993,19 +7039,19 @@
       </c>
       <c r="F238" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G238" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H238" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I238" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="239" spans="3:9" x14ac:dyDescent="0.25">
@@ -7017,19 +7063,19 @@
       </c>
       <c r="F239" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G239" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H239" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I239" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="240" spans="3:9" x14ac:dyDescent="0.25">
@@ -7041,19 +7087,19 @@
       </c>
       <c r="F240" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G240" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H240" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I240" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="241" spans="3:9" x14ac:dyDescent="0.25">
@@ -7065,19 +7111,19 @@
       </c>
       <c r="F241" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G241" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H241" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I241" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="242" spans="3:9" x14ac:dyDescent="0.25">
@@ -7089,19 +7135,19 @@
       </c>
       <c r="F242" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G242" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H242" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I242" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="243" spans="3:9" x14ac:dyDescent="0.25">
@@ -7113,19 +7159,19 @@
       </c>
       <c r="F243" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G243" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H243" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I243" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="244" spans="3:9" x14ac:dyDescent="0.25">
@@ -7137,19 +7183,19 @@
       </c>
       <c r="F244" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G244" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H244" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I244" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="245" spans="3:9" x14ac:dyDescent="0.25">
@@ -7161,19 +7207,19 @@
       </c>
       <c r="F245" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G245" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H245" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I245" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="246" spans="3:9" x14ac:dyDescent="0.25">
@@ -7185,19 +7231,19 @@
       </c>
       <c r="F246" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G246" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H246" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I246" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="247" spans="3:9" x14ac:dyDescent="0.25">
@@ -7209,19 +7255,19 @@
       </c>
       <c r="F247" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G247" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H247" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I247" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="248" spans="3:9" x14ac:dyDescent="0.25">
@@ -7233,19 +7279,19 @@
       </c>
       <c r="F248" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G248" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H248" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I248" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="249" spans="3:9" x14ac:dyDescent="0.25">
@@ -7257,19 +7303,19 @@
       </c>
       <c r="F249" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G249" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H249" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I249" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="250" spans="3:9" x14ac:dyDescent="0.25">
@@ -7281,19 +7327,19 @@
       </c>
       <c r="F250" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G250" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H250" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I250" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="251" spans="3:9" x14ac:dyDescent="0.25">
@@ -7305,19 +7351,19 @@
       </c>
       <c r="F251" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G251" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H251" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I251" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="252" spans="3:9" x14ac:dyDescent="0.25">
@@ -7329,19 +7375,19 @@
       </c>
       <c r="F252" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G252" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H252" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I252" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="253" spans="3:9" x14ac:dyDescent="0.25">
@@ -7353,19 +7399,19 @@
       </c>
       <c r="F253" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G253" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H253" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I253" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="254" spans="3:9" x14ac:dyDescent="0.25">
@@ -7377,19 +7423,19 @@
       </c>
       <c r="F254" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G254" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H254" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I254" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
     <row r="255" spans="3:9" x14ac:dyDescent="0.25">
@@ -7401,19 +7447,19 @@
       </c>
       <c r="F255" s="13">
         <f t="shared" si="25"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="G255" s="8">
         <f t="shared" si="26"/>
-        <v>3.9159722222222211</v>
+        <v>4.2472222222222209</v>
       </c>
       <c r="H255" s="8">
         <f t="shared" si="27"/>
-        <v>5.0659722222222214</v>
+        <v>5.397222222222223</v>
       </c>
       <c r="I255" s="15">
         <f t="shared" si="28"/>
-        <v>20669.166666666664</v>
+        <v>22020.666666666672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>